<commit_message>
atualização para o NodeJS
</commit_message>
<xml_diff>
--- a/icons/criador de ícones.xlsx
+++ b/icons/criador de ícones.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Desktop\SUSEP_teste\webapp\old\icons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73B9167-481A-46EC-A1B8-9C6CC268CE5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929A4387-159F-4C67-8866-E4E0FF71DF76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="8505" windowHeight="10305" xr2:uid="{B0E6DA6B-EAD3-48EA-B90A-3D2D3F9F2351}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B0E6DA6B-EAD3-48EA-B90A-3D2D3F9F2351}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Auto</t>
   </si>
@@ -49,7 +50,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,13 +58,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF004D86"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -88,8 +103,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF004D86"/>
+      <color rgb="FF00192D"/>
       <color rgb="FFC00000"/>
-      <color rgb="FF004D86"/>
       <color rgb="FF00B050"/>
     </mruColors>
   </colors>
@@ -105,6 +121,414 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16354177602799649"/>
+          <c:y val="8.7763713080168781E-2"/>
+          <c:w val="0.68680555555555556"/>
+          <c:h val="0.8345991561181435"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004D86"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="2"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7F1A-4BFF-9490-6FF74C293761}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004D86"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7F1A-4BFF-9490-6FF74C293761}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7F1A-4BFF-9490-6FF74C293761}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Planilha1 (2)'!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Auto</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Vida</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Outros</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Planilha1 (2)'!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-7F1A-4BFF-9490-6FF74C293761}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="121"/>
+        <c:holeSize val="60"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.5384099351798271E-2"/>
+          <c:y val="8.7763713080168781E-2"/>
+          <c:w val="0.83590048049105681"/>
+          <c:h val="0.8345991561181435"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="41275" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:tailEnd type="triangle"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Planilha1 (2)'!$H$2:$M$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Planilha1 (2)'!$H$3:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CEE0-422B-8B16-59FCBF575432}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="30"/>
+        <c:axId val="388919096"/>
+        <c:axId val="388919424"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="388919096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="388919424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="388919424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="65"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="388919096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
@@ -299,7 +723,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
@@ -592,6 +1016,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -1630,7 +2134,3475 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>354139</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="Fundo Azul">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23027A69-CA60-413C-BA58-D840ADD9918B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13696950" y="3105150"/>
+          <a:ext cx="1897189" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="004D86"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>18106</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="22" name="Agrupar 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D8C9C8-C9E8-482B-871F-9E1372F25150}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks noChangeAspect="1"/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13861930" y="3104971"/>
+          <a:ext cx="1661663" cy="1819409"/>
+          <a:chOff x="11770427" y="6394451"/>
+          <a:chExt cx="2093822" cy="2705100"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="23" name="perguntadores" descr="Perguntas com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F522632-61E7-4EED-9253-F0487C726CAC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect l="12915" t="8358" r="13018" b="8462"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11770427" y="6394451"/>
+            <a:ext cx="2093822" cy="2705100"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="fundo azul apoio Info">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7C7F80-FE6D-4538-A7C6-380539E7B5DB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="12885116" y="6487136"/>
+            <a:ext cx="742186" cy="848026"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln w="28575">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="25" name="Gráfico 24" descr="Informações com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBE1CD9B-641D-491C-AD55-6608FAAC7C47}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="12895096" y="6534352"/>
+            <a:ext cx="754342" cy="743563"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8030BB1A-0AAE-4BF1-8D13-B68AC602CEE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADBD285B-4F50-4D8A-8D17-7E2BC2B58FD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Retângulo 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC6F7587-3458-4EA2-BA28-419CE08B379B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7581901" y="2095500"/>
+          <a:ext cx="1009650" cy="981075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>22224</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>75142</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>502707</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>17992</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Agrupar 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8748F305-BABD-4D96-B1BE-839C4FAB062A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="22224" y="6491038"/>
+          <a:ext cx="2924634" cy="2584690"/>
+          <a:chOff x="8915400" y="1190625"/>
+          <a:chExt cx="2286000" cy="2286000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="9" name="Gráfico 8" descr="Papel estrutura de tópicos">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{310D8AE7-C6A4-442A-9DF3-3F5DB9A00B43}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8915400" y="1190625"/>
+            <a:ext cx="2286000" cy="2286000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="10" name="Gráfico 9" descr="Balança da justiça com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45815CEB-6EBB-4455-B1B9-F3780699A0E7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId10"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9519365" y="1470740"/>
+            <a:ext cx="522294" cy="522294"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="11" name="Gráfico 10" descr="Gráfico de barras com tendência ascendente com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FF331AB-1094-4A5E-A757-C7C893B7B88C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId12"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect l="24174" t="6956" r="10400" b="21591"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9597343" y="2126002"/>
+            <a:ext cx="918257" cy="1002833"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>27050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>17525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Gráfico 11" descr="Dinheiro estrutura de tópicos">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01C5482C-2F63-4F23-BE97-D43AE4B46A0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId14"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8905874" y="1352549"/>
+          <a:ext cx="2093976" cy="2093976"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>35094</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>100262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>105278</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>65506</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="13" name="Agrupar 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42B8342D-89A2-47B5-B9C3-60A61DEEC643}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks noChangeAspect="1"/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5534434" y="1609885"/>
+          <a:ext cx="1903297" cy="1852272"/>
+          <a:chOff x="5838164" y="1702742"/>
+          <a:chExt cx="1551712" cy="1227881"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="14" name="Gráfico 13" descr="Moedas estrutura de tópicos">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB3F5D45-1992-4844-A79A-6B337BF4E6F1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId16"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect l="8264" t="13174" r="4539" b="12517"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="6580040" y="2337223"/>
+            <a:ext cx="809836" cy="593400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="15" name="Gráfico 14" descr="Balança da justiça com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB9E2B57-3BEE-4646-8A99-E68710E3DF31}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId17"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect l="6732" t="7241" r="7541" b="7090"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5838164" y="1702742"/>
+            <a:ext cx="1223249" cy="871841"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190842</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>187253</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>250087</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>184205</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="16" name="Agrupar 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66303669-7616-4647-8EE0-FE856C8A0F69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6301219" y="4150012"/>
+          <a:ext cx="1892359" cy="1883981"/>
+          <a:chOff x="7589274" y="5361649"/>
+          <a:chExt cx="3072582" cy="3041859"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="Retângulo 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{786C060B-10DE-4E20-BDB4-D002E6A0676D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7589274" y="6882581"/>
+            <a:ext cx="906412" cy="1520926"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="004D86"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="3200">
+                <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>2</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="Retângulo 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4403B20-D0E5-4B38-9386-62DD97CD84CB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8672359" y="6275746"/>
+            <a:ext cx="906412" cy="2127761"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="004D86"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="3200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>1</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="3200">
+              <a:effectLst/>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="Retângulo 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66BBBFC7-D080-47C5-9A57-BCC30459F645}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9755443" y="7274978"/>
+            <a:ext cx="906413" cy="1128530"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="004D86"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="3200">
+                <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>3</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="20" name="Gráfico 19" descr="Troféu com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C34BA1A7-7B89-458D-AEA9-D68A2AE171F9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId19"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8680042" y="5361649"/>
+            <a:ext cx="914400" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="21" name="Gráfico 20" descr="Estrela com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07DD0831-4613-4DBF-9EA0-F816B7A4F5E3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId21"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9027791" y="5486643"/>
+            <a:ext cx="218900" cy="218900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>370139</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>17714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>591812</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>86987</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Gráfico 26" descr="Moedas com preenchimento sólido">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29BBA6BB-B6E0-4938-B01A-1E44FF4A59B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId23"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13171739" y="8018714"/>
+          <a:ext cx="831273" cy="831273"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>250606</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>68792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>137582</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>104743</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="28" name="Agrupar 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8674554-4F50-4DCC-86E1-0EDBE5FC62DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3916832" y="6484688"/>
+          <a:ext cx="2942165" cy="1922980"/>
+          <a:chOff x="3732524" y="7087026"/>
+          <a:chExt cx="2921437" cy="1904527"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="29" name="Gráfico 28" descr="Livro aberto estrutura de tópicos">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F60FB822-8C9C-44A1-B52D-92ED41D7D9F9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId25"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect t="16288" b="19328"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3732524" y="7087026"/>
+            <a:ext cx="2921437" cy="1880933"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="30" name="Gráfico 29" descr="Lupa com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D54FEB8E-1F3F-4257-98E2-C13C9992ADAA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId27"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4002497" y="7209646"/>
+            <a:ext cx="1781907" cy="1781907"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="31" name="Gráfico 30" descr="Fluxograma com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3401B602-CC2D-4481-86F4-29A41D1C14DB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId29"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4277613" y="7441220"/>
+            <a:ext cx="900375" cy="896888"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>455083</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>105834</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342060</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>117740</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="32" name="Agrupar 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6DD7A90-D035-4E3A-8EB3-70B6A82BC460}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7176498" y="6521730"/>
+          <a:ext cx="2942166" cy="1898935"/>
+          <a:chOff x="7207250" y="6582834"/>
+          <a:chExt cx="2956143" cy="1916906"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="33" name="Gráfico 32" descr="Livro aberto estrutura de tópicos">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D7F38D4-C8FC-4FAE-BC51-14A6E54CF81A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId25"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect t="16288" b="19328"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7207250" y="6582834"/>
+            <a:ext cx="2956143" cy="1916906"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="34" name="Agrupar 33">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F30AF59-7F9F-4134-9861-54D78921F4CD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="7768167" y="6720417"/>
+            <a:ext cx="867059" cy="1322371"/>
+            <a:chOff x="6752167" y="8763000"/>
+            <a:chExt cx="867059" cy="1322371"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="36" name="Gráfico 35" descr="Mecânico de Automóveis com preenchimento sólido">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1442D8C-18A8-4FDF-955B-19323FF30452}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill rotWithShape="1">
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId31"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:srcRect t="29819" b="-1"/>
+            <a:stretch/>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7173894" y="8831150"/>
+              <a:ext cx="445332" cy="311102"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="37" name="Gráfico 36" descr="Cofrinho com preenchimento sólido">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{102D8300-70D1-4726-95FD-B8E10F2BF4E7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId33"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7173894" y="9163745"/>
+              <a:ext cx="445332" cy="447063"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="38" name="Gráfico 37" descr="Fábrica com preenchimento sólido">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{695DF525-691E-40FD-80E4-B67618F57ADD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId35"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6752167" y="9605539"/>
+              <a:ext cx="445333" cy="479832"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="39" name="Gráfico 38" descr="Início com preenchimento sólido">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22D3BF2A-F6C7-447C-9BAC-63586A3003D7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId37"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6767856" y="8763000"/>
+              <a:ext cx="404848" cy="401307"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="40" name="Gráfico 39" descr="Homem com carrinho de bebê com preenchimento sólido">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20F0144A-8A85-476D-89AA-D5E93749E2EB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId39"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6772409" y="9185554"/>
+              <a:ext cx="404848" cy="401307"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="41" name="Gráfico 40" descr="Médico com preenchimento sólido">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF5BB26A-9BA2-42AB-830C-3249EA7641F4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId41"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7173894" y="9621254"/>
+              <a:ext cx="445332" cy="441436"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="35" name="Gráfico 34" descr="Lupa com preenchimento sólido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC2623C-C827-4076-BCA1-66A63FE69AFC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId27"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="8062515" y="6601969"/>
+            <a:ext cx="1803076" cy="1815986"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>148165</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>169334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>551578</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>169334</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="42" name="Agrupar 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB35205D-6E32-45B4-9661-BFD7A373A4B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks noChangeAspect="1"/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6869580" y="8849664"/>
+          <a:ext cx="1625489" cy="1887028"/>
+          <a:chOff x="7001520" y="8995292"/>
+          <a:chExt cx="2070605" cy="2418339"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="43" name="Gráfico 42" descr="Prancheta Parcialmente Marcada estrutura de tópicos">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{928F17F0-C6FB-4FBA-AD43-0C9DFFD80658}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId43"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect l="17830" t="7303" r="17949" b="7271"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7396676" y="8995292"/>
+            <a:ext cx="1675449" cy="2228666"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="44" name="Agrupar 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37989A80-0B41-4E7E-A862-6FFD34E3CCB2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="7001520" y="10050208"/>
+            <a:ext cx="1166420" cy="1363423"/>
+            <a:chOff x="5466937" y="9563375"/>
+            <a:chExt cx="1166420" cy="1363423"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="45" name="Retângulo 44">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1392CFF6-C29A-4B00-BA0E-6DA8A2371373}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5556249" y="9768416"/>
+              <a:ext cx="687917" cy="1079500"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent6"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent6"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="46" name="Gráfico 45" descr="Calculadora com preenchimento sólido">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB685C6F-7D8D-43E8-8D34-6C00C824ADC1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill rotWithShape="1">
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId45"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:srcRect l="20795" b="7417"/>
+            <a:stretch/>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5466937" y="9563375"/>
+              <a:ext cx="1166420" cy="1363423"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>412751</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>42335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Imagem 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FC3698D-AACD-44A2-853E-EBEAABFD690E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:srcRect l="16217" t="15916" r="14492" b="14498"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1631951" y="9948333"/>
+          <a:ext cx="1892300" cy="1905002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>42333</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>102785</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Imagem 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56DADDEA-BA97-4C32-A9DD-9A6D19BFC9F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:srcRect l="10628" t="11340" r="8773" b="7532"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2480733" y="3566583"/>
+          <a:ext cx="1889252" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Imagem 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E16C85F-F368-435F-AE94-D77DA1F42AF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1209675" cy="1514475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>314168</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>385889</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161466</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="63" name="Agrupar 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{896ECFA5-A5B0-46BE-AACA-C4FE712B432A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13756998" y="708983"/>
+          <a:ext cx="1904834" cy="1905620"/>
+          <a:chOff x="13760293" y="714375"/>
+          <a:chExt cx="1905284" cy="1923591"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="50" name="Fundo Azul">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ED83580-0561-4ED1-8E91-D4F56B8E5A05}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="13763625" y="714375"/>
+            <a:ext cx="1901952" cy="1905000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="004D86"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="62" name="Agrupar 61">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{155738C2-E808-42D0-A438-507ED9D28C78}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="13760293" y="730251"/>
+            <a:ext cx="1896990" cy="1907715"/>
+            <a:chOff x="13760293" y="730251"/>
+            <a:chExt cx="1896990" cy="1907715"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="3" name="Mundo" descr="Globo terrestre: Américas com preenchimento sólido">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBEDA489-902E-4D60-8EE4-9772D6928BE2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill rotWithShape="1">
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId50"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:srcRect l="10090" t="10089" r="9814" b="9814"/>
+            <a:stretch/>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13760293" y="730251"/>
+              <a:ext cx="1896990" cy="1887930"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="61" name="Agrupar 60">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{128FC823-5B66-46F4-8EDF-43171C1B6DF4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="13771838" y="1610078"/>
+              <a:ext cx="819182" cy="1027888"/>
+              <a:chOff x="13771838" y="1610078"/>
+              <a:chExt cx="819182" cy="1027888"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="4" name="Saco de Dinheiro">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B67AF569-AAD4-428B-93A8-BB14B9EF9D0A}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51">
+                <a:biLevel thresh="50000"/>
+                <a:extLst>
+                  <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                    <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                      <a14:imgLayer r:embed="rId52">
+                        <a14:imgEffect>
+                          <a14:backgroundRemoval t="5660" b="96855" l="3150" r="93701">
+                            <a14:foregroundMark x1="61417" y1="43396" x2="85827" y2="71069"/>
+                            <a14:foregroundMark x1="85827" y1="71069" x2="84252" y2="79874"/>
+                            <a14:foregroundMark x1="74803" y1="92453" x2="32283" y2="93711"/>
+                            <a14:foregroundMark x1="32283" y1="93711" x2="18110" y2="63522"/>
+                            <a14:foregroundMark x1="3150" y1="83019" x2="3150" y2="76101"/>
+                            <a14:foregroundMark x1="44882" y1="56604" x2="44882" y2="56604"/>
+                            <a14:foregroundMark x1="93701" y1="77358" x2="92913" y2="82390"/>
+                            <a14:foregroundMark x1="55906" y1="26415" x2="68504" y2="12579"/>
+                            <a14:foregroundMark x1="46457" y1="9434" x2="38583" y2="6289"/>
+                            <a14:foregroundMark x1="65354" y1="96855" x2="31496" y2="96226"/>
+                            <a14:foregroundMark x1="53543" y1="74843" x2="53543" y2="74843"/>
+                            <a14:foregroundMark x1="60630" y1="54717" x2="37008" y2="76730"/>
+                            <a14:foregroundMark x1="42520" y1="61006" x2="66142" y2="74214"/>
+                            <a14:foregroundMark x1="38583" y1="61006" x2="45669" y2="51572"/>
+                            <a14:foregroundMark x1="45669" y1="51572" x2="60630" y2="54717"/>
+                            <a14:foregroundMark x1="56693" y1="57233" x2="44094" y2="85535"/>
+                          </a14:backgroundRemoval>
+                        </a14:imgEffect>
+                      </a14:imgLayer>
+                    </a14:imgProps>
+                  </a:ext>
+                </a:extLst>
+              </a:blip>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="13771838" y="1610078"/>
+                <a:ext cx="819182" cy="1027888"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="52" name="Cifrão" descr="Dólar com preenchimento sólido">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26C1EF15-CD66-4345-BFB9-936E3D66E94E}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53">
+                <a:extLst>
+                  <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                    <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                  </a:ext>
+                  <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                    <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId54"/>
+                  </a:ext>
+                </a:extLst>
+              </a:blip>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="13928897" y="2033336"/>
+                <a:ext cx="505065" cy="503656"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+        </xdr:grpSp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>249394</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>317783</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="74" name="Agrupar 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0608905-B81B-4666-8DE6-82E3F455836F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="16136375" y="661358"/>
+          <a:ext cx="1901502" cy="1887029"/>
+          <a:chOff x="16140269" y="666750"/>
+          <a:chExt cx="1901952" cy="1905000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="64" name="Agrupar 63">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1565849A-F68A-4693-AF60-855DFDD05050}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="16140269" y="666750"/>
+            <a:ext cx="1901952" cy="1905000"/>
+            <a:chOff x="13763625" y="714375"/>
+            <a:chExt cx="1901952" cy="1905000"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="65" name="Fundo Azul">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9498A706-0A88-4079-B17A-5584BB39FDCE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13763625" y="714375"/>
+              <a:ext cx="1901952" cy="1905000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="004D86"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="70" name="Cifrão" descr="Dólar com preenchimento sólido">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023CB33C-FDED-4BBA-818E-9B2E9EF863EA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+                <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                  <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId54"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13928897" y="2033336"/>
+              <a:ext cx="505065" cy="503656"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="71" name="Retângulo: Cantos Arredondados 70">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41EFEADA-9D1C-43DF-A0CA-BE3B918DE514}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16396714" y="934400"/>
+            <a:ext cx="1389063" cy="274324"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="72" name="Retângulo: Cantos Arredondados 71">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEB0A445-D38E-417E-AC59-4E4674094A17}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16396714" y="1486056"/>
+            <a:ext cx="1389063" cy="274324"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="73" name="Retângulo: Cantos Arredondados 72">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1982284-3A26-4C06-BED6-CD3E678C0314}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16396714" y="2037712"/>
+            <a:ext cx="1389063" cy="274324"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="pt-BR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3914,10 +7886,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D564A1A8-0705-4EFE-8B32-138AC7F5FCA2}">
+  <dimension ref="A2:U12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="Q1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>2000</v>
+      </c>
+      <c r="I2">
+        <f>H2+1</f>
+        <v>2001</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:M2" si="0">I2+1</f>
+        <v>2002</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>17.5</v>
+      </c>
+      <c r="J3">
+        <v>35</v>
+      </c>
+      <c r="K3">
+        <v>25</v>
+      </c>
+      <c r="L3">
+        <v>47</v>
+      </c>
+      <c r="M3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B90ED7-FE25-463B-8C96-885467ACE07B}">
   <dimension ref="A2:M5"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="H15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="H15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>

</xml_diff>